<commit_message>
took out useless functions and updated my weekly reports
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/WillertzTimeCard.xlsx
+++ b/YellowLib/YellowLib/WillertzTimeCard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willertz_n\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willertz_n\Source\Repos\Yellow Project\YellowLib\YellowLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="20">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -638,8 +638,8 @@
   </sheetPr>
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -715,11 +715,11 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
@@ -747,11 +747,11 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
+      <c r="B8" s="4">
+        <v>43506</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
@@ -759,20 +759,19 @@
       <c r="E8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
+      <c r="F8" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G8" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
+      <c r="B9" s="4">
+        <v>43508</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.79166666666666663</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>12</v>
@@ -780,20 +779,19 @@
       <c r="E9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>14</v>
+      <c r="F9" s="6">
+        <v>0.875</v>
       </c>
       <c r="G9" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>11</v>
+      <c r="B10" s="4">
+        <v>43513</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>12</v>
@@ -801,20 +799,19 @@
       <c r="E10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>14</v>
+      <c r="F10" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G10" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>11</v>
+      <c r="B11" s="4">
+        <v>43515</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.75</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>12</v>
@@ -822,12 +819,12 @@
       <c r="E11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>14</v>
+      <c r="F11" s="6">
+        <v>0.83333333333333337</v>
       </c>
       <c r="G11" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated timecard and reports
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/WillertzTimeCard.xlsx
+++ b/YellowLib/YellowLib/WillertzTimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="20">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -638,8 +638,8 @@
   </sheetPr>
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -715,11 +715,11 @@
       </c>
       <c r="C6" s="3">
         <f>SUBTOTAL(109,TimeSheet[Hours Worked])</f>
-        <v>8</v>
+        <v>9.9999999999999982</v>
       </c>
       <c r="D6" s="3">
         <f>IFERROR(IF(C6&lt;=WorkweekHours,C6,WorkweekHours),"")</f>
-        <v>8</v>
+        <v>9.9999999999999982</v>
       </c>
       <c r="E6" s="3">
         <f>IFERROR(C6-D6, "")</f>
@@ -828,11 +828,11 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>11</v>
+      <c r="B12" s="4">
+        <v>43520</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>12</v>
@@ -840,20 +840,20 @@
       <c r="E12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>14</v>
+      <c r="F12" s="6">
+        <v>0.66666666666666663</v>
       </c>
       <c r="G12" s="5">
         <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
+      <c r="B13" s="4">
+        <v>43522</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.75</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>12</v>
@@ -861,20 +861,19 @@
       <c r="E13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
+      <c r="F13" s="6">
+        <v>0.83333333333333337</v>
       </c>
       <c r="G13" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
+      <c r="B14" s="4">
+        <v>43527</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.58333333333333337</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>12</v>
@@ -882,20 +881,19 @@
       <c r="E14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>14</v>
+      <c r="F14" s="6">
+        <v>0.70833333333333337</v>
       </c>
       <c r="G14" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>11</v>
+      <c r="B15" s="4">
+        <v>43529</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.75</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>12</v>
@@ -903,12 +901,11 @@
       <c r="E15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>14</v>
+      <c r="F15" s="6">
+        <v>0.875</v>
       </c>
       <c r="G15" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working on reading in xml
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/WillertzTimeCard.xlsx
+++ b/YellowLib/YellowLib/WillertzTimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="32">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>11:15AM</t>
+  </si>
+  <si>
+    <t>7:15PM</t>
+  </si>
+  <si>
+    <t>10:00AM</t>
+  </si>
+  <si>
+    <t>11:00M</t>
   </si>
 </sst>
 </file>
@@ -666,7 +675,7 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1076,11 +1085,11 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>16</v>
+      <c r="B23" s="4">
+        <v>43559</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>12</v>
@@ -1089,19 +1098,18 @@
         <v>13</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G23" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>16</v>
+      <c r="B24" s="4">
+        <v>43564</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>12</v>
@@ -1110,19 +1118,18 @@
         <v>13</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G24" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>16</v>
+      <c r="B25" s="4">
+        <v>43566</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>12</v>
@@ -1131,11 +1138,10 @@
         <v>13</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="G25" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated weekly report and tcard
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/WillertzTimeCard.xlsx
+++ b/YellowLib/YellowLib/WillertzTimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="33">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>11:00M</t>
+  </si>
+  <si>
+    <t>4:30PM</t>
   </si>
 </sst>
 </file>
@@ -674,8 +677,8 @@
   </sheetPr>
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1145,11 +1148,11 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>16</v>
+      <c r="B26" s="4">
+        <v>43569</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>12</v>
@@ -1158,11 +1161,10 @@
         <v>13</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G26" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated report and tcard
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/WillertzTimeCard.xlsx
+++ b/YellowLib/YellowLib/WillertzTimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="34">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>4:30PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:00PM </t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1168,11 +1171,11 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>16</v>
+      <c r="B27" s="4">
+        <v>43571</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>12</v>
@@ -1181,11 +1184,10 @@
         <v>13</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G27" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated timecard and weekly report
</commit_message>
<xml_diff>
--- a/YellowLib/YellowLib/WillertzTimeCard.xlsx
+++ b/YellowLib/YellowLib/WillertzTimeCard.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
   <si>
     <t>Time Sheet</t>
   </si>
@@ -681,7 +681,7 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1191,11 +1191,11 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>16</v>
+      <c r="B28" s="4">
+        <v>43576</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>12</v>
@@ -1204,19 +1204,18 @@
         <v>13</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G28" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>16</v>
+      <c r="B29" s="4">
+        <v>43578</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>12</v>
@@ -1225,19 +1224,18 @@
         <v>13</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G29" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>16</v>
+      <c r="B30" s="4">
+        <v>43585</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>12</v>
@@ -1246,11 +1244,10 @@
         <v>13</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G30" s="5">
-        <f>IFERROR(IF(COUNT(TimeSheet[[#This Row],[Time In]:[Time Out]])=4,(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Lunch End]]+TimeSheet[[#This Row],[Lunch Start]]-TimeSheet[[#This Row],[Time In]],IF(AND(LEN(TimeSheet[[#This Row],[Time In]])&lt;&gt;0,LEN(TimeSheet[[#This Row],[Time Out]])&lt;&gt;0),(IF(TimeSheet[[#This Row],[Time Out]]&lt;TimeSheet[[#This Row],[Time In]],1,0)+TimeSheet[[#This Row],[Time Out]])-TimeSheet[[#This Row],[Time In]],0))*24,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>